<commit_message>
tutorial finished. Working as intended. Now, work on modifying it to fit your needs, teppy.
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
@@ -1448,6 +1448,101 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="B51" t="n">
+        <v>44</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>try again</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>33</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>agaaaiiiinnn</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>22</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>patrick</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>45</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>lloyd</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>25</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
misc uploads. file refenrences. added ttkboostrap to reqs
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
@@ -1543,6 +1543,86 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>teppppppp</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>22</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>33</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>patrick</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>44</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>asdfasdfasdfasdfjklhasdfkjlashdf</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>44</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added edit rows thru double-clicks, Added delete row option, Moved status indicator to bottom, Improved date validation and display (removed timestamps), Auto-focus on newly-added rows now reimplemented (accidentally removed before)
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="11310" yWindow="1890" windowWidth="16140" windowHeight="13365" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -53,9 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,17 +436,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.44140625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="16.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="16.77734375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -467,19 +470,24 @@
           <t>Employment</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,15 +499,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -511,15 +519,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>Alice Wong</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -531,35 +539,35 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alice Wong</t>
+          <t>Mark Lee</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mark Lee</t>
+          <t>Emily Chen</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -571,31 +579,31 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Emily Chen</t>
+          <t>David Kim</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>David Kim</t>
+          <t>Karen Wu</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -611,15 +619,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Karen Wu</t>
+          <t>Tom Brown</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -631,51 +639,51 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tom Brown</t>
+          <t>Lisa Park</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lisa Park</t>
+          <t>Michael Kim</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Michael Kim</t>
+          <t>Sarah Lee</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -691,55 +699,55 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sarah Lee</t>
+          <t>Eric Wang</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Eric Wang</t>
+          <t>Michelle Chu</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Michelle Chu</t>
+          <t>Jake Lee</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -751,15 +759,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jake Lee</t>
+          <t>Anna Kim</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -771,11 +779,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Anna Kim</t>
+          <t>Brian Yu</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -791,51 +799,51 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Brian Yu</t>
+          <t>Mary Lee</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mary Lee</t>
+          <t>Peter Lee</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Peter Lee</t>
+          <t>Grace Lee</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -851,15 +859,15 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Grace Lee</t>
+          <t>Joshua Chen</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -871,15 +879,15 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Joshua Chen</t>
+          <t>Amy Huang</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -891,15 +899,15 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Amy Huang</t>
+          <t>Chris Chang</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -911,11 +919,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Chris Chang</t>
+          <t>Tina Wu</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -931,55 +939,55 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Tina Wu</t>
+          <t>Daniel Kim</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Daniel Kim</t>
+          <t>Lisa Lee</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lisa Lee</t>
+          <t>Samuel Choi</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -991,15 +999,15 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Samuel Choi</t>
+          <t>Rachel Kim</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1011,11 +1019,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Rachel Kim</t>
+          <t>Jason Han</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1031,15 +1039,15 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Jason Han</t>
+          <t>Erica Park</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1051,15 +1059,15 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Erica Park</t>
+          <t>Danny Cho</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1071,15 +1079,15 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Danny Cho</t>
+          <t>Katie Kim</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1091,15 +1099,15 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Katie Kim</t>
+          <t>Oliver Lee</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1111,51 +1119,51 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Oliver Lee</t>
+          <t>Hannah Lee</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Hannah Lee</t>
+          <t>Alex Kim</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Alex Kim</t>
+          <t>Cindy Lim</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1171,51 +1179,51 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Cindy Lim</t>
+          <t>Timothy Lee</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Timothy Lee</t>
+          <t>Kelly Kim</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Kelly Kim</t>
+          <t>David Lee</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1231,15 +1239,15 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>David Lee</t>
+          <t>Julie Kim</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1251,15 +1259,15 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Julie Kim</t>
+          <t>Steven Yoon</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1271,11 +1279,11 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Steven Yoon</t>
+          <t>Sophia Kim</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1291,15 +1299,15 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sophia Kim</t>
+          <t>Jason Lee</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1311,15 +1319,15 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Jason Lee</t>
+          <t>Evelyn Kim</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1331,11 +1339,11 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Evelyn Kim</t>
+          <t>Ryan Park</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1351,15 +1359,15 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Ryan Park</t>
+          <t>Megan Lee</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1371,11 +1379,11 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Megan Lee</t>
+          <t>JT</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1391,27 +1399,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>JT</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>jkihgjhf</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1419,58 +1427,58 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="n">
+        <v>44</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>try again</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>33</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>Unemployed</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>jkihgjhf</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>24</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Employed</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="n">
-        <v>44</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Not Subscribed</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>try again</t>
+          <t>agaaaiiiinnn</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1479,38 +1487,38 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>agaaaiiiinnn</t>
+          <t>patrick</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>patrick</t>
+          <t>lloyd</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1519,18 +1527,18 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Employed</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>lloyd</t>
+          <t>teppppppp</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1546,11 +1554,11 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>teppppppp</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1559,22 +1567,22 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Unemployed</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>patrick</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>Not Subscribed</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1586,7 +1594,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>patrick</t>
+          <t>asdfasdfasdfasdfjklhasdfkjlashdf</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1594,7 +1602,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Not Subscribed</t>
+          <t>Subscribed</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1606,32 +1614,34 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>asdfasdfasdfasdfjklhasdfkjlashdf</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>44</v>
+          <t>teppy</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Subscribed</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Permanent</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>teppy</t>
+          <t>another</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>33</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1641,74 +1651,53 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Permanent</t>
+          <t>permanent</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>another</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+          <t>aayayy</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>55</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>asdfasdf</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>permanent</t>
+          <t>asdfasdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>aayayy</t>
+          <t>new row</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
+          <t>owyeah</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>asdfasdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>last</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>2</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-    </row>
-    <row r="64"/>
-    <row r="65"/>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>45718</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
added togglers for required fields and duplicate policies
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -57,11 +56,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +445,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="16.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
@@ -455,7 +453,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name  (unique)</t>
+          <t>Name [warn]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -738,7 +736,7 @@
           <t>Employed</t>
         </is>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="2" t="n">
         <v>45689</v>
       </c>
     </row>
@@ -1725,6 +1723,191 @@
       </c>
       <c r="E63" s="2" t="n">
         <v>45871</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>cindy lim2</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>jlkasdf</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>45909</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025/1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-1-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>25/1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ v4.3.0 — Excel-style workflow & numeric intelligence upgrade
- Added Excel-like keyboard shortcuts (Ctrl+O/S/N/D/F2, etc.)
- Insert, delete, and duplicate rows with visual flash animations
- Duplicate rows now auto-increment ID-like fields (ID001 → ID002)
- Implemented header-aware numeric rules:
  • amount/price/rate fields rounded to 2 decimals
  • other numeric fields default to integer display
- Added universal spreadsheet support (.xlsm, .xlsb, .xls, .ods)
- Improved UI polish, validation consistency, and auto-save safety
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -56,10 +57,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,13 +439,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
@@ -1864,22 +1866,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>25/1/1</t>
         </is>
       </c>
     </row>
@@ -1891,23 +1893,123 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>1</t>
         </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>12</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>afds</t>
+        </is>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>45658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ UI/UX Overhaul: Added floating Help Card, improved toolbar layout, and modernized Excel-style status bar.
- Added Help Card reading from help.txt (scrollable, themed window)
- Added ❓ Help button beside Theme selector with tooltip + hover
- Grouped Auto-Save, Theme, Help controls in right-aligned toolbar cluster
- Introduced unified tooltip and hover behavior for all toolbar controls
- Replaced old status bar with color-coded, right-aligned version featuring fade-out transitions
- Minor styling cleanup and readiness for future Markdown help support
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,6 +761,9 @@
           <t>Employed</t>
         </is>
       </c>
+      <c r="E15" s="3" t="n">
+        <v>45658</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2009,6 +2012,26 @@
         </is>
       </c>
       <c r="E74" s="3" t="n">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>patrick</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>aadsf</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>asdfasdf</t>
+        </is>
+      </c>
+      <c r="E75" s="3" t="n">
         <v>45658</v>
       </c>
     </row>

</xml_diff>